<commit_message>
Implement cache for performance increase
</commit_message>
<xml_diff>
--- a/quotes.xlsx
+++ b/quotes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\PycharmProjects\conferences\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BA49C1A-A67E-4EF4-BA4E-29303889B494}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B3CE726-08A3-4978-9DFA-FCC0EAE1D3D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{DC629059-7EB7-405E-82F5-1FE29D7ADC8F}"/>
+    <workbookView xWindow="28680" yWindow="105" windowWidth="29040" windowHeight="16440" xr2:uid="{DC629059-7EB7-405E-82F5-1FE29D7ADC8F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="163">
   <si>
     <t>Author</t>
   </si>
@@ -441,10 +441,6 @@
     <t>Les mathématiques sont le squelette du monde, la physique en est la chair.</t>
   </si>
   <si>
-    <t xml:space="preserve">Noir ! J'ai besoin d'obscurité, de rester seul dans le noir. La chambre des enfants, volets fermés, très bien. La régularisation. Le schéma de Newton. Les constantes exponentielles. Tout virevolte dans ma tête.
-Juste après avoir ramené les enfants à la maison, je suis allé me réfugier dans ma chambre, pour continuer à remuer mes pensées. Demain c'est mon exposé à Rutgers, et la preuve ne tient toujours pas debout. J'ai besoin de marcher en solitaire pour réfléchir. Il y urgence ! </t>
-  </si>
-  <si>
     <t>Les sciences font partie de ce qui engendre le monde du futur. C'est un devoir que les femmes y soient associées de façon très importante. Sinon, quel est le message ? Le message qu'on renvoie, ça veut dire que c'est aux hommes d'enfanter le futur. Ça c'est un message qui est inadmissible.</t>
   </si>
   <si>
@@ -530,9 +526,6 @@
     <t xml:space="preserve">L'amour est cette confiance faite au hasard. </t>
   </si>
   <si>
-    <t xml:space="preserve">... l'amour, comme toute procédure de vérité, est essentiellement désintéressé : sa valeur ne réside qu'en lui-même, et cette valeur est au-delà des intérêts immédiats des deux individus qui y sont engagés. </t>
-  </si>
-  <si>
     <t xml:space="preserve">Les difficultés de l'amour ne tiennent pas à l'existence d'un ennemi identifié. Elles sont internes à son processus : le jeu créateur de la différence. C'est l'égoïsme qui est l'ennemi de l'amour, non le rival. On pourrait dire : l'ennemi principal de mon amour, celui que je dois vaincre, ce n'est pas l'autre, c'est moi, le "moi" qui veut l'identité contre la différence, qui veut imposer son mode contre le monde filtré et reconstruit dans le prisme de la différence. </t>
   </si>
   <si>
@@ -545,10 +538,13 @@
     <t>Un amour véritable est celui qui triomphe durablement, parfois durement, des obstacles que l'espace, le monde et le temps lui proposent.</t>
   </si>
   <si>
-    <t>Les autres</t>
-  </si>
-  <si>
-    <t>L'enfer, c'est nous</t>
+    <t>Alain Gourvest</t>
+  </si>
+  <si>
+    <t>On nous dit sans arrêt "Nul n'est censé ignorer la loi." Laquelle loi ? Il y en a des milliers, des millions, écrites par les hommes. Ce n'est pas faisable. L a notion de faisabilité est une notion importante en systémique. Nous ferions beaucoup mieux de dire "Nul n'est censé ignoré les finalités des lois." Et là il y en a beaucoup moins.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L'amour, comme toute procédure de vérité, est essentiellement désintéressé : sa valeur ne réside qu'en lui-même, et cette valeur est au-delà des intérêts immédiats des deux individus qui y sont engagés. </t>
   </si>
 </sst>
 </file>
@@ -909,10 +905,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4284B3C1-4664-4D64-B17E-B7860122B00D}">
-  <dimension ref="A1:B151"/>
+  <dimension ref="A1:B150"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A136" workbookViewId="0">
-      <selection activeCell="B154" sqref="B154"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2002,15 +1998,15 @@
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>125</v>
+        <v>146</v>
       </c>
       <c r="B136" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B137" t="s">
         <v>148</v>
@@ -2018,7 +2014,7 @@
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B138" t="s">
         <v>149</v>
@@ -2026,7 +2022,7 @@
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B139" t="s">
         <v>150</v>
@@ -2034,7 +2030,7 @@
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B140" t="s">
         <v>151</v>
@@ -2042,7 +2038,7 @@
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B141" t="s">
         <v>152</v>
@@ -2050,7 +2046,7 @@
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B142" t="s">
         <v>153</v>
@@ -2058,7 +2054,7 @@
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B143" t="s">
         <v>154</v>
@@ -2066,7 +2062,7 @@
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B144" t="s">
         <v>155</v>
@@ -2074,58 +2070,50 @@
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B145" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B146" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B147" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B148" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B149" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>147</v>
+        <v>160</v>
       </c>
       <c r="B150" t="s">
         <v>161</v>
-      </c>
-    </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A151" t="s">
-        <v>162</v>
-      </c>
-      <c r="B151" t="s">
-        <v>163</v>
       </c>
     </row>
   </sheetData>

</xml_diff>